<commit_message>
refactoring (problem files & misc)
</commit_message>
<xml_diff>
--- a/data/vehicules.xlsx
+++ b/data/vehicules.xlsx
@@ -34,7 +34,7 @@
     <t>Frais Contrôle Technique (€/an)</t>
   </si>
   <si>
-    <t>Frais Assurance (€/mois)</t>
+    <t>Frais Assurance (€/an)</t>
   </si>
   <si>
     <t>Frais Entretien (€/km)</t>
@@ -112,12 +112,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -126,13 +129,16 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -443,14 +449,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="23.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="27.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="23.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="27.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="29.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -475,320 +481,320 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>9000</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>10</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4">
-        <v>120</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="F2" s="5">
+        <v>150</v>
+      </c>
+      <c r="G2" s="5">
+        <v>750</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.0384</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
+        <v>4000</v>
+      </c>
+      <c r="C3" s="5">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5">
         <v>15</v>
       </c>
-      <c r="H2" s="5">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4">
-        <v>4000</v>
-      </c>
-      <c r="C3" s="4">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4">
-        <v>100</v>
-      </c>
-      <c r="G3" s="4">
-        <v>15</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0.18</v>
+      <c r="F3" s="5">
+        <v>150</v>
+      </c>
+      <c r="G3" s="5">
+        <v>750</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.0384</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>1400</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>4</v>
       </c>
-      <c r="D4" s="4">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="4">
-        <v>80</v>
-      </c>
-      <c r="G4" s="4">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.09</v>
+      <c r="D4" s="5">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5">
+        <v>80</v>
+      </c>
+      <c r="G4" s="5">
+        <v>500</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>1400</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4">
-        <v>80</v>
-      </c>
-      <c r="G5" s="4">
-        <v>15</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.09</v>
+      <c r="D5" s="5">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5">
+        <v>80</v>
+      </c>
+      <c r="G5" s="5">
+        <v>500</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>1400</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="4">
-        <v>80</v>
-      </c>
-      <c r="G6" s="4">
-        <v>15</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.09</v>
+      <c r="D6" s="5">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5">
+        <v>80</v>
+      </c>
+      <c r="G6" s="5">
+        <v>500</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>1400</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="4">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4">
-        <v>80</v>
-      </c>
-      <c r="G7" s="4">
-        <v>15</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.09</v>
+      <c r="D7" s="5">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5">
+        <v>80</v>
+      </c>
+      <c r="G7" s="5">
+        <v>500</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>1400</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="4">
-        <v>12</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="4">
-        <v>80</v>
-      </c>
-      <c r="G8" s="4">
-        <v>15</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.09</v>
+      <c r="D8" s="5">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5">
+        <v>80</v>
+      </c>
+      <c r="G8" s="5">
+        <v>500</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>1400</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>4</v>
       </c>
-      <c r="D9" s="4">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4">
-        <v>80</v>
-      </c>
-      <c r="G9" s="4">
-        <v>15</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.09</v>
+      <c r="D9" s="5">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5">
+        <v>80</v>
+      </c>
+      <c r="G9" s="5">
+        <v>500</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <v>1400</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>4</v>
       </c>
-      <c r="D10" s="4">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="4">
-        <v>80</v>
-      </c>
-      <c r="G10" s="4">
-        <v>15</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0.09</v>
+      <c r="D10" s="5">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5">
+        <v>80</v>
+      </c>
+      <c r="G10" s="5">
+        <v>500</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="5">
         <v>1600</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>3</v>
       </c>
-      <c r="D11" s="4">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="5">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="4">
-        <v>80</v>
-      </c>
-      <c r="G11" s="4">
-        <v>15</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0.09</v>
+      <c r="F11" s="5">
+        <v>80</v>
+      </c>
+      <c r="G11" s="5">
+        <v>500</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5">
         <v>1600</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>3</v>
       </c>
-      <c r="D12" s="4">
-        <v>12</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="5">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="4">
-        <v>80</v>
-      </c>
-      <c r="G12" s="4">
-        <v>15</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0.09</v>
+      <c r="F12" s="5">
+        <v>80</v>
+      </c>
+      <c r="G12" s="5">
+        <v>500</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.0186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="5">
         <v>1600</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>3</v>
       </c>
-      <c r="D13" s="4">
-        <v>12</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="5">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="4">
-        <v>80</v>
-      </c>
-      <c r="G13" s="4">
-        <v>15</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.09</v>
+      <c r="F13" s="5">
+        <v>80</v>
+      </c>
+      <c r="G13" s="5">
+        <v>500</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.0186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>